<commit_message>
Fixed data.json and report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/DEDALUS/4C_Suite/6.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/DEDALUS/4C_Suite/6.1/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/enrico_badolati_dedalus_eu/Documents/Documenti/FSE2.0/test/DEDALUS/4C_Suite/6.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="407" documentId="8_{9809B93C-B7DE-463E-A796-84FADBB93DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDA49B0B-167E-4A7A-A187-4EF407186E2D}"/>
+  <xr:revisionPtr revIDLastSave="412" documentId="8_{9809B93C-B7DE-463E-A796-84FADBB93DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E7E3090-B42C-4480-AFB1-F4AE1B4973B2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -847,15 +847,6 @@
 </t>
   </si>
   <si>
-    <t>8a3987e67895c21a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.524da43d04975eefc9278377dbf86cdc13925be8aa313ec7ec6d58c1b3d84538.859b83fcf5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-10T15:44:06Z</t>
-  </si>
-  <si>
     <t>741ee6e347695e2d</t>
   </si>
   <si>
@@ -1037,6 +1028,15 @@
   </si>
   <si>
     <t>subject_application_version: 6.1</t>
+  </si>
+  <si>
+    <t>2023-06-10T15:42:05Z</t>
+  </si>
+  <si>
+    <t>5227af8c3043a64c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.524da43d04975eefc9278377dbf86cdc13925be8aa313ec7ec6d58c1b3d84538.dab5f37de2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1046,11 +1046,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1460,76 +1467,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1538,7 +1545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1562,61 +1569,64 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4081,10 +4091,10 @@
   <dimension ref="A1:T378"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N29" sqref="N29"/>
+      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4122,14 +4132,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4147,14 +4157,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="58" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="50"/>
+      <c r="D3" s="51"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4172,12 +4182,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="58" t="s">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4196,12 +4206,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="59" t="s">
-        <v>240</v>
-      </c>
-      <c r="D5" s="50"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" s="51"/>
       <c r="E5" s="46"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -4220,8 +4230,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4670,13 +4680,13 @@
         <v>45202</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I17" s="37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J17" s="31" t="s">
         <v>55</v>
@@ -4689,7 +4699,7 @@
         <v>55</v>
       </c>
       <c r="N17" s="31" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O17" s="31" t="s">
         <v>55</v>
@@ -4726,13 +4736,13 @@
         <v>45202</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I18" s="37" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J18" s="31" t="s">
         <v>55</v>
@@ -4745,7 +4755,7 @@
         <v>55</v>
       </c>
       <c r="N18" s="31" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O18" s="31" t="s">
         <v>55</v>
@@ -4782,13 +4792,13 @@
         <v>45202</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I19" s="37" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J19" s="31" t="s">
         <v>55</v>
@@ -4801,7 +4811,7 @@
         <v>55</v>
       </c>
       <c r="N19" s="31" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O19" s="31" t="s">
         <v>55</v>
@@ -4838,13 +4848,13 @@
         <v>45202</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I20" s="37" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J20" s="31" t="s">
         <v>55</v>
@@ -4857,7 +4867,7 @@
         <v>55</v>
       </c>
       <c r="N20" s="31" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O20" s="31" t="s">
         <v>55</v>
@@ -4894,13 +4904,13 @@
         <v>45203</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H21" s="37" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I21" s="37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J21" s="31" t="s">
         <v>55</v>
@@ -4913,7 +4923,7 @@
         <v>55</v>
       </c>
       <c r="N21" s="31" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O21" s="31" t="s">
         <v>55</v>
@@ -4950,13 +4960,13 @@
         <v>45203</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I22" s="37" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J22" s="31" t="s">
         <v>55</v>
@@ -4969,7 +4979,7 @@
         <v>55</v>
       </c>
       <c r="N22" s="31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O22" s="31" t="s">
         <v>55</v>
@@ -5006,13 +5016,13 @@
         <v>45203</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J23" s="31" t="s">
         <v>55</v>
@@ -5025,7 +5035,7 @@
         <v>55</v>
       </c>
       <c r="N23" s="31" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O23" s="31" t="s">
         <v>55</v>
@@ -5062,13 +5072,13 @@
         <v>45203</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H24" s="37" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I24" s="37" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J24" s="31" t="s">
         <v>55</v>
@@ -5081,7 +5091,7 @@
         <v>55</v>
       </c>
       <c r="N24" s="31" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O24" s="31" t="s">
         <v>55</v>
@@ -5118,13 +5128,13 @@
         <v>45203</v>
       </c>
       <c r="G25" s="37" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H25" s="37" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I25" s="37" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J25" s="31" t="s">
         <v>55</v>
@@ -5137,7 +5147,7 @@
         <v>55</v>
       </c>
       <c r="N25" s="31" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="O25" s="31" t="s">
         <v>55</v>
@@ -5174,13 +5184,13 @@
         <v>45203</v>
       </c>
       <c r="G26" s="37" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I26" s="37" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J26" s="31" t="s">
         <v>55</v>
@@ -5193,7 +5203,7 @@
         <v>55</v>
       </c>
       <c r="N26" s="31" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="O26" s="31" t="s">
         <v>55</v>
@@ -5230,13 +5240,13 @@
         <v>45203</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I27" s="37" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J27" s="31" t="s">
         <v>55</v>
@@ -5249,7 +5259,7 @@
         <v>55</v>
       </c>
       <c r="N27" s="31" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="O27" s="31" t="s">
         <v>55</v>
@@ -5286,13 +5296,13 @@
         <v>45203</v>
       </c>
       <c r="G28" s="37" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H28" s="37" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I28" s="37" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J28" s="31" t="s">
         <v>55</v>
@@ -5305,7 +5315,7 @@
         <v>55</v>
       </c>
       <c r="N28" s="31" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="O28" s="31" t="s">
         <v>55</v>
@@ -5342,13 +5352,13 @@
         <v>45203</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H29" s="45" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I29" s="45" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J29" s="31" t="s">
         <v>55</v>
@@ -5361,9 +5371,9 @@
         <v>55</v>
       </c>
       <c r="N29" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="O29" s="60" t="s">
+        <v>234</v>
+      </c>
+      <c r="O29" s="47" t="s">
         <v>55</v>
       </c>
       <c r="P29" s="20" t="s">
@@ -5550,13 +5560,13 @@
         <v>45203</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H34" s="37" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I34" s="37" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J34" s="31" t="s">
         <v>55</v>
@@ -5569,7 +5579,7 @@
         <v>55</v>
       </c>
       <c r="N34" s="31" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O34" s="31" t="s">
         <v>55</v>
@@ -5606,13 +5616,13 @@
         <v>45203</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H35" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I35" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J35" s="31" t="s">
         <v>55</v>
@@ -5625,7 +5635,7 @@
         <v>55</v>
       </c>
       <c r="N35" s="31" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="O35" s="31" t="s">
         <v>55</v>
@@ -5662,13 +5672,13 @@
         <v>45202</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="H36" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="I36" s="25" t="s">
-        <v>178</v>
+        <v>239</v>
+      </c>
+      <c r="I36" s="61" t="s">
+        <v>240</v>
       </c>
       <c r="J36" s="26" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Fixed test case 0 - id 374
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/DEDALUS/4C_Suite/6.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/DEDALUS/4C_Suite/6.1/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/enrico_badolati_dedalus_eu/Documents/Documenti/FSE2.0/test/DEDALUS/4C_Suite/6.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="412" documentId="8_{9809B93C-B7DE-463E-A796-84FADBB93DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E7E3090-B42C-4480-AFB1-F4AE1B4973B2}"/>
+  <xr:revisionPtr revIDLastSave="415" documentId="8_{9809B93C-B7DE-463E-A796-84FADBB93DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FC091BE-0E83-4D9A-B9C6-3156BC550023}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1030,13 +1030,13 @@
     <t>subject_application_version: 6.1</t>
   </si>
   <si>
-    <t>2023-06-10T15:42:05Z</t>
-  </si>
-  <si>
-    <t>5227af8c3043a64c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.524da43d04975eefc9278377dbf86cdc13925be8aa313ec7ec6d58c1b3d84538.dab5f37de2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-11-10T14:28:11Z</t>
+  </si>
+  <si>
+    <t>0669fcc622e8a641</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.524da43d04975eefc9278377dbf86cdc13925be8aa313ec7ec6d58c1b3d84538.d4759823dd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1533,9 +1533,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1600,6 +1597,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1624,9 +1624,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4091,10 +4088,10 @@
   <dimension ref="A1:T378"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
+      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4212,7 +4209,7 @@
         <v>237</v>
       </c>
       <c r="D5" s="51"/>
-      <c r="E5" s="46"/>
+      <c r="E5" s="45"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4349,1352 +4346,1352 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
+      <c r="A10" s="26">
         <v>32</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="29">
         <v>45202</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31" t="s">
+      <c r="K10" s="30"/>
+      <c r="L10" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M10" s="31" t="s">
+      <c r="M10" s="30" t="s">
         <v>55</v>
       </c>
       <c r="N10" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="O10" s="31" t="s">
+      <c r="O10" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P10" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q10" s="31" t="s">
+      <c r="Q10" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R10" s="32"/>
-      <c r="S10" s="33"/>
-      <c r="T10" s="34" t="s">
+      <c r="R10" s="31"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27">
+      <c r="A11" s="26">
         <v>40</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="29">
         <v>45202</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="J11" s="31" t="s">
+      <c r="J11" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31" t="s">
+      <c r="K11" s="30"/>
+      <c r="L11" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M11" s="31" t="s">
+      <c r="M11" s="30" t="s">
         <v>55</v>
       </c>
       <c r="N11" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="O11" s="31" t="s">
+      <c r="O11" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P11" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q11" s="31" t="s">
+      <c r="Q11" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R11" s="32"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="34" t="s">
+      <c r="R11" s="31"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="A12" s="26">
         <v>48</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31" t="s">
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M12" s="31" t="s">
+      <c r="M12" s="30" t="s">
         <v>55</v>
       </c>
       <c r="N12" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="O12" s="31" t="s">
+      <c r="O12" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P12" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q12" s="31" t="s">
+      <c r="Q12" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R12" s="32" t="s">
+      <c r="R12" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="S12" s="33"/>
-      <c r="T12" s="34" t="s">
+      <c r="S12" s="32"/>
+      <c r="T12" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27">
+      <c r="A13" s="26">
         <v>147</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31" t="s">
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="K13" s="31" t="s">
+      <c r="K13" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="33"/>
-      <c r="T13" s="34" t="s">
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
+      <c r="A14" s="26">
         <v>148</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="31" t="s">
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="K14" s="31" t="s">
+      <c r="K14" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="33"/>
-      <c r="T14" s="34" t="s">
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27">
+      <c r="A15" s="26">
         <v>149</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31" t="s">
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="34" t="s">
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
+      <c r="A16" s="26">
         <v>150</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="31" t="s">
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="K16" s="31" t="s">
+      <c r="K16" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="34" t="s">
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27">
+      <c r="A17" s="26">
         <v>151</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="29">
         <v>45202</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="H17" s="37" t="s">
+      <c r="H17" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="I17" s="37" t="s">
+      <c r="I17" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J17" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31" t="s">
+      <c r="K17" s="30"/>
+      <c r="L17" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M17" s="31" t="s">
+      <c r="M17" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N17" s="31" t="s">
+      <c r="N17" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="O17" s="31" t="s">
+      <c r="O17" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P17" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q17" s="31" t="s">
+      <c r="Q17" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R17" s="32"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="34" t="s">
+      <c r="R17" s="31"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27">
+      <c r="A18" s="26">
         <v>152</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="29">
         <v>45202</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G18" s="36" t="s">
         <v>211</v>
       </c>
-      <c r="H18" s="37" t="s">
+      <c r="H18" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="I18" s="37" t="s">
+      <c r="I18" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31" t="s">
+      <c r="K18" s="30"/>
+      <c r="L18" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M18" s="31" t="s">
+      <c r="M18" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N18" s="31" t="s">
+      <c r="N18" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="O18" s="31" t="s">
+      <c r="O18" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P18" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q18" s="31" t="s">
+      <c r="Q18" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R18" s="32"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="34" t="s">
+      <c r="R18" s="31"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27">
+      <c r="A19" s="26">
         <v>153</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="29">
         <v>45202</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="I19" s="37" t="s">
+      <c r="I19" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="J19" s="31" t="s">
+      <c r="J19" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31" t="s">
+      <c r="K19" s="30"/>
+      <c r="L19" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M19" s="31" t="s">
+      <c r="M19" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N19" s="31" t="s">
+      <c r="N19" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="O19" s="31" t="s">
+      <c r="O19" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P19" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q19" s="31" t="s">
+      <c r="Q19" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R19" s="32"/>
-      <c r="S19" s="33"/>
-      <c r="T19" s="34" t="s">
+      <c r="R19" s="31"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27">
+      <c r="A20" s="26">
         <v>154</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="29">
         <v>45202</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="36" t="s">
         <v>213</v>
       </c>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="J20" s="31" t="s">
+      <c r="J20" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31" t="s">
+      <c r="K20" s="30"/>
+      <c r="L20" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M20" s="31" t="s">
+      <c r="M20" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N20" s="31" t="s">
+      <c r="N20" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="O20" s="31" t="s">
+      <c r="O20" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P20" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q20" s="31" t="s">
+      <c r="Q20" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R20" s="32"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="34" t="s">
+      <c r="R20" s="31"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27">
+      <c r="A21" s="26">
         <v>155</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="29">
         <v>45203</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="H21" s="37" t="s">
+      <c r="H21" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="I21" s="37" t="s">
+      <c r="I21" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="J21" s="31" t="s">
+      <c r="J21" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31" t="s">
+      <c r="K21" s="30"/>
+      <c r="L21" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M21" s="31" t="s">
+      <c r="M21" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N21" s="31" t="s">
+      <c r="N21" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="O21" s="31" t="s">
+      <c r="O21" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P21" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q21" s="31" t="s">
+      <c r="Q21" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R21" s="32"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="34" t="s">
+      <c r="R21" s="31"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27">
+      <c r="A22" s="26">
         <v>156</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="29">
         <v>45203</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="H22" s="37" t="s">
+      <c r="H22" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="I22" s="37" t="s">
+      <c r="I22" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="J22" s="31" t="s">
+      <c r="J22" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31" t="s">
+      <c r="K22" s="30"/>
+      <c r="L22" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M22" s="31" t="s">
+      <c r="M22" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N22" s="31" t="s">
+      <c r="N22" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="O22" s="31" t="s">
+      <c r="O22" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P22" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q22" s="31" t="s">
+      <c r="Q22" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R22" s="32"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="34" t="s">
+      <c r="R22" s="31"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27">
+      <c r="A23" s="26">
         <v>157</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="35" t="s">
+      <c r="E23" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="29">
         <v>45203</v>
       </c>
-      <c r="G23" s="37" t="s">
+      <c r="G23" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="H23" s="37" t="s">
+      <c r="H23" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="I23" s="37" t="s">
+      <c r="I23" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="J23" s="31" t="s">
+      <c r="J23" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31" t="s">
+      <c r="K23" s="30"/>
+      <c r="L23" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M23" s="31" t="s">
+      <c r="M23" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N23" s="31" t="s">
+      <c r="N23" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="O23" s="31" t="s">
+      <c r="O23" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P23" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q23" s="31" t="s">
+      <c r="Q23" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R23" s="32"/>
-      <c r="S23" s="33"/>
-      <c r="T23" s="34" t="s">
+      <c r="R23" s="31"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27">
+      <c r="A24" s="26">
         <v>158</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="F24" s="30">
+      <c r="F24" s="29">
         <v>45203</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="H24" s="37" t="s">
+      <c r="H24" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="I24" s="37" t="s">
+      <c r="I24" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="J24" s="31" t="s">
+      <c r="J24" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31" t="s">
+      <c r="K24" s="30"/>
+      <c r="L24" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M24" s="31" t="s">
+      <c r="M24" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N24" s="31" t="s">
+      <c r="N24" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="O24" s="31" t="s">
+      <c r="O24" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P24" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q24" s="31" t="s">
+      <c r="Q24" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R24" s="32"/>
-      <c r="S24" s="33"/>
-      <c r="T24" s="34" t="s">
+      <c r="R24" s="31"/>
+      <c r="S24" s="32"/>
+      <c r="T24" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27">
+      <c r="A25" s="26">
         <v>159</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="E25" s="35" t="s">
+      <c r="E25" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="29">
         <v>45203</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="H25" s="37" t="s">
+      <c r="H25" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="I25" s="37" t="s">
+      <c r="I25" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="J25" s="31" t="s">
+      <c r="J25" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31" t="s">
+      <c r="K25" s="30"/>
+      <c r="L25" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M25" s="31" t="s">
+      <c r="M25" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N25" s="31" t="s">
+      <c r="N25" s="30" t="s">
         <v>230</v>
       </c>
-      <c r="O25" s="31" t="s">
+      <c r="O25" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P25" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q25" s="31" t="s">
+      <c r="Q25" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R25" s="32"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="34" t="s">
+      <c r="R25" s="31"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27">
+      <c r="A26" s="26">
         <v>160</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="F26" s="30">
+      <c r="F26" s="29">
         <v>45203</v>
       </c>
-      <c r="G26" s="37" t="s">
+      <c r="G26" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="H26" s="37" t="s">
+      <c r="H26" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="I26" s="37" t="s">
+      <c r="I26" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="J26" s="31" t="s">
+      <c r="J26" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31" t="s">
+      <c r="K26" s="30"/>
+      <c r="L26" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M26" s="31" t="s">
+      <c r="M26" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N26" s="31" t="s">
+      <c r="N26" s="30" t="s">
         <v>231</v>
       </c>
-      <c r="O26" s="31" t="s">
+      <c r="O26" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P26" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q26" s="31" t="s">
+      <c r="Q26" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R26" s="32"/>
-      <c r="S26" s="33"/>
-      <c r="T26" s="34" t="s">
+      <c r="R26" s="31"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="27">
+      <c r="A27" s="26">
         <v>161</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="F27" s="30">
+      <c r="F27" s="29">
         <v>45203</v>
       </c>
-      <c r="G27" s="37" t="s">
+      <c r="G27" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="H27" s="37" t="s">
+      <c r="H27" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="I27" s="37" t="s">
+      <c r="I27" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="J27" s="31" t="s">
+      <c r="J27" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31" t="s">
+      <c r="K27" s="30"/>
+      <c r="L27" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M27" s="31" t="s">
+      <c r="M27" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N27" s="31" t="s">
+      <c r="N27" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="O27" s="31" t="s">
+      <c r="O27" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P27" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q27" s="31" t="s">
+      <c r="Q27" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R27" s="32"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="34" t="s">
+      <c r="R27" s="31"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="27">
+      <c r="A28" s="26">
         <v>162</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="E28" s="35" t="s">
+      <c r="E28" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="29">
         <v>45203</v>
       </c>
-      <c r="G28" s="37" t="s">
+      <c r="G28" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="H28" s="37" t="s">
+      <c r="H28" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="I28" s="37" t="s">
+      <c r="I28" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31" t="s">
+      <c r="K28" s="30"/>
+      <c r="L28" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M28" s="31" t="s">
+      <c r="M28" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N28" s="31" t="s">
+      <c r="N28" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="O28" s="31" t="s">
+      <c r="O28" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P28" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q28" s="31" t="s">
+      <c r="Q28" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R28" s="32"/>
-      <c r="S28" s="33"/>
-      <c r="T28" s="34" t="s">
+      <c r="R28" s="31"/>
+      <c r="S28" s="32"/>
+      <c r="T28" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="27">
+      <c r="A29" s="26">
         <v>163</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="F29" s="30">
+      <c r="F29" s="29">
         <v>45203</v>
       </c>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="H29" s="45" t="s">
+      <c r="H29" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="I29" s="45" t="s">
+      <c r="I29" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="J29" s="31" t="s">
+      <c r="J29" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31" t="s">
+      <c r="K29" s="30"/>
+      <c r="L29" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M29" s="31" t="s">
+      <c r="M29" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N29" s="31" t="s">
+      <c r="N29" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="O29" s="47" t="s">
+      <c r="O29" s="46" t="s">
         <v>55</v>
       </c>
       <c r="P29" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q29" s="31" t="s">
+      <c r="Q29" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R29" s="32"/>
-      <c r="S29" s="33"/>
-      <c r="T29" s="34" t="s">
+      <c r="R29" s="31"/>
+      <c r="S29" s="32"/>
+      <c r="T29" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27">
+      <c r="A30" s="26">
         <v>164</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="F30" s="30"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="31" t="s">
+      <c r="F30" s="29"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="K30" s="31" t="s">
+      <c r="K30" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="31"/>
-      <c r="R30" s="32"/>
-      <c r="S30" s="33"/>
-      <c r="T30" s="34" t="s">
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27">
+      <c r="A31" s="26">
         <v>165</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="F31" s="30"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="31" t="s">
+      <c r="F31" s="29"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="K31" s="31" t="s">
+      <c r="K31" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="31"/>
-      <c r="Q31" s="31"/>
-      <c r="R31" s="32"/>
-      <c r="S31" s="33"/>
-      <c r="T31" s="34" t="s">
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="31"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="27">
+      <c r="A32" s="26">
         <v>166</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="31" t="s">
+      <c r="F32" s="29"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="K32" s="31" t="s">
+      <c r="K32" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="32"/>
-      <c r="S32" s="33"/>
-      <c r="T32" s="34" t="s">
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="27">
+      <c r="A33" s="26">
         <v>167</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="31" t="s">
+      <c r="F33" s="29"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="K33" s="31" t="s">
+      <c r="K33" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
-      <c r="Q33" s="31"/>
-      <c r="R33" s="32"/>
-      <c r="S33" s="33"/>
-      <c r="T33" s="34" t="s">
+      <c r="L33" s="30"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="30"/>
+      <c r="O33" s="30"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="30"/>
+      <c r="R33" s="31"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27">
+      <c r="A34" s="26">
         <v>168</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="F34" s="30">
+      <c r="F34" s="29">
         <v>45203</v>
       </c>
-      <c r="G34" s="37" t="s">
+      <c r="G34" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="H34" s="37" t="s">
+      <c r="H34" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="I34" s="37" t="s">
+      <c r="I34" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="J34" s="31" t="s">
+      <c r="J34" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31" t="s">
+      <c r="K34" s="30"/>
+      <c r="L34" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M34" s="31" t="s">
+      <c r="M34" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N34" s="31" t="s">
+      <c r="N34" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="O34" s="31" t="s">
+      <c r="O34" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P34" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q34" s="31" t="s">
+      <c r="Q34" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R34" s="32"/>
-      <c r="S34" s="33"/>
-      <c r="T34" s="34" t="s">
+      <c r="R34" s="31"/>
+      <c r="S34" s="32"/>
+      <c r="T34" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27">
+      <c r="A35" s="26">
         <v>169</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="E35" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="F35" s="30">
+      <c r="F35" s="29">
         <v>45203</v>
       </c>
-      <c r="G35" s="37" t="s">
+      <c r="G35" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="H35" s="37" t="s">
+      <c r="H35" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="I35" s="37" t="s">
+      <c r="I35" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="J35" s="31" t="s">
+      <c r="J35" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31" t="s">
+      <c r="K35" s="30"/>
+      <c r="L35" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="M35" s="31" t="s">
+      <c r="M35" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N35" s="31" t="s">
+      <c r="N35" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="O35" s="31" t="s">
+      <c r="O35" s="30" t="s">
         <v>55</v>
       </c>
       <c r="P35" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="Q35" s="31" t="s">
+      <c r="Q35" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R35" s="32"/>
-      <c r="S35" s="33"/>
-      <c r="T35" s="34" t="s">
+      <c r="R35" s="31"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="38">
+      <c r="A36" s="37">
         <v>374</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="39" t="s">
+      <c r="D36" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="F36" s="41">
+      <c r="F36" s="40">
         <v>45202</v>
       </c>
-      <c r="G36" s="25" t="s">
+      <c r="G36" s="47" t="s">
         <v>238</v>
       </c>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="I36" s="61" t="s">
+      <c r="I36" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="J36" s="26" t="s">
+      <c r="J36" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="26"/>
-      <c r="Q36" s="31" t="s">
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="R36" s="42"/>
-      <c r="S36" s="43"/>
-      <c r="T36" s="44" t="s">
+      <c r="R36" s="41"/>
+      <c r="S36" s="42"/>
+      <c r="T36" s="43" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed report-checklist and data.json
Fixed report-checklist and data.json
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/DEDALUS/4C_Suite/6.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/DEDALUS/4C_Suite/6.1/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/enrico_badolati_dedalus_eu/Documents/Documenti/FSE2.0/test/DEDALUS/4C_Suite/6.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enrico.badolati\OneDrive - Dedalus S.p.A\Documenti\FSE2.0\test\DEDALUS\4C_Suite\6.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="415" documentId="8_{9809B93C-B7DE-463E-A796-84FADBB93DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FC091BE-0E83-4D9A-B9C6-3156BC550023}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B699C11-CE06-42C3-841E-1723872B99F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -826,18 +826,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-10-03T15:30:15Z</t>
-  </si>
-  <si>
-    <t>aacbb29b6c106f46</t>
-  </si>
-  <si>
-    <t>8662455c40b51845</t>
-  </si>
-  <si>
-    <t>2023-10-03T15:31:27Z</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RSA_CT0</t>
   </si>
   <si>
@@ -847,141 +835,6 @@
 </t>
   </si>
   <si>
-    <t>741ee6e347695e2d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.64a31cbb7433730b03d21b732a017cb45334e7d5c40865d3f1f0a9a6ca2a439e.8cf499a679^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-10-03T15:45:58Z</t>
-  </si>
-  <si>
-    <t>d10199275531e749</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.ed671d263d5d22d8e682d5c980b503f4f789557b7851c216b58f98e8b006cf9b.a946a2ef79^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6d5a7db4875a347d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.24e373daac1a42d317e650d4e74c704600dbf25ecb592cc74cdabbe7a74753cd.a0af9b57f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>30405ef4e12ac92f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.20d0cf61e1f8afd29000d4a17ae64d52784c629e267bce6eccd75c371df45783.b1b60b92c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e9fba503590b640f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.761baf080e69d64ef55a3ee1fb24715bc4db9bdbfebf22ced2ed001958c7bc38.8b49e059b8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>d5ad0f98b9bc8cbc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.c8ff979203ed76d1111ac84d3d3c5b2a81fbb16171c9c641ad6076a18def78fd.57ff949f78^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>027751beb3755042</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.543ec699ef8825cdd2eee88b64ddfee23c9c8b0093ff472bb9645c8b52847ed3.d9c009aa5e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>1ffa01cd5b3637a5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.86551093341555ba9bf9764420ff53a1e8093a4026d1d12fb17ff05c035b488b.509f1b6e2c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>88d02396e02164dc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.014e71b9ab133b0509002617359a8dff2148c324dbdfc78d3b0f51e47fda233e.4ccc305522^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-07-03T07:58:37Z</t>
-  </si>
-  <si>
-    <t>dd8c46054d607b15</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.ec85690b05c0eee98616fea896e58cf5e6105940d1d984bfc7f48bf899e77b65.e9d3aaf7e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>027c90b629900d57</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.51bfc25f81560704afc0ef640d8439d0f5dd3bda0e39d0a71ee269e2990cc4c6.8ca8d0e642^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>b2befedfad139a23</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.cc7fd2230f1e86a36c7c7a155fcb99332cb6e598acb4200a6d85e3ae0e64b1f7.26836b9b8e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>81b8c3a63cdb416e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.9b109b8ee8248f573873f6c576744756db2f2b6246e53dcefc9eef35be4a19d8.1dd82835a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>56e03d1bdccc4c19</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.8099e0f23406b2c671fb582747c436c6618820907e301f43002735c4cb50cd41.e2edb82c70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-10-04T08:04:43Z</t>
-  </si>
-  <si>
-    <t>9a6fad2137250e1e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.d7b0ac4bd81058ada7ed526c7dc7fe5ca60b6b3e977964fb3a8f0e10cad178e8.67ac9f675b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-10-04T08:06:04Z</t>
-  </si>
-  <si>
-    <t>2023-10-03T15:50:20Z</t>
-  </si>
-  <si>
-    <t>2023-10-03T15:51:20Z</t>
-  </si>
-  <si>
-    <t>2023-10-03T15:52:40Z</t>
-  </si>
-  <si>
-    <t>2023-10-04T07:53:38Z</t>
-  </si>
-  <si>
-    <t>2023-10-04T07:54:46Z</t>
-  </si>
-  <si>
-    <t>2023-10-04T07:55:49Z</t>
-  </si>
-  <si>
-    <t>2023-10-04T07:57:31Z</t>
-  </si>
-  <si>
-    <t>2023-10-04T08:25:30Z</t>
-  </si>
-  <si>
-    <t>2023-10-04T08:00:39Z</t>
-  </si>
-  <si>
-    <t>2023-10-04T08:01:55Z</t>
-  </si>
-  <si>
-    <t>2023-10-04T08:03:15Z</t>
-  </si>
-  <si>
     <t>"ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected."</t>
   </si>
   <si>
@@ -1030,13 +883,160 @@
     <t>subject_application_version: 6.1</t>
   </si>
   <si>
-    <t>2023-11-10T14:28:11Z</t>
-  </si>
-  <si>
-    <t>0669fcc622e8a641</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120103.4.4.524da43d04975eefc9278377dbf86cdc13925be8aa313ec7ec6d58c1b3d84538.d4759823dd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>495b3d3de2c41043</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.524da43d04975eefc9278377dbf86cdc13925be8aa313ec7ec6d58c1b3d84538.7f0968833b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-16T08:56:25Z</t>
+  </si>
+  <si>
+    <t>2023-10-16T08:59:46Z</t>
+  </si>
+  <si>
+    <t>34f1ff64a025f489</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.64a31cbb7433730b03d21b732a017cb45334e7d5c40865d3f1f0a9a6ca2a439e.e38cd80655^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:08:07Z</t>
+  </si>
+  <si>
+    <t>08d6188b2fab8511</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.ed671d263d5d22d8e682d5c980b503f4f789557b7851c216b58f98e8b006cf9b.901243b8e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:09:35Z</t>
+  </si>
+  <si>
+    <t>89383eb25e111624</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.24e373daac1a42d317e650d4e74c704600dbf25ecb592cc74cdabbe7a74753cd.048b35b7e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:11:04Z</t>
+  </si>
+  <si>
+    <t>b311fc619c875ddb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.20d0cf61e1f8afd29000d4a17ae64d52784c629e267bce6eccd75c371df45783.ca3dc2450a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b0f9fc7442b7b9bd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.761baf080e69d64ef55a3ee1fb24715bc4db9bdbfebf22ced2ed001958c7bc38.02384ad529^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:13:45Z</t>
+  </si>
+  <si>
+    <t>0d87bfda84106f44</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.c8ff979203ed76d1111ac84d3d3c5b2a81fbb16171c9c641ad6076a18def78fd.7ff49fb1b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:15:12Z</t>
+  </si>
+  <si>
+    <t>122bc18662f431d4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.543ec699ef8825cdd2eee88b64ddfee23c9c8b0093ff472bb9645c8b52847ed3.c65213045d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>d2cb38a99eb9b736</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.86551093341555ba9bf9764420ff53a1e8093a4026d1d12fb17ff05c035b488b.ce9c9c29b5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.014e71b9ab133b0509002617359a8dff2148c324dbdfc78d3b0f51e47fda233e.5a88c21b31^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3f535352825c2421</t>
+  </si>
+  <si>
+    <t>087b1a7336de85a1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.ec85690b05c0eee98616fea896e58cf5e6105940d1d984bfc7f48bf899e77b65.6d5fe77763^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b735c7b23c0e910b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.51bfc25f81560704afc0ef640d8439d0f5dd3bda0e39d0a71ee269e2990cc4c6.b5806c72ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>56c4e45b6a1f412c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.cc7fd2230f1e86a36c7c7a155fcb99332cb6e598acb4200a6d85e3ae0e64b1f7.1501431083^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9b019012413bff7d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.9b109b8ee8248f573873f6c576744756db2f2b6246e53dcefc9eef35be4a19d8.c7916fbdb7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8790933fe71d15f3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.8099e0f23406b2c671fb582747c436c6618820907e301f43002735c4cb50cd41.48db821c47^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4a17d08ce7637f53</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120103.4.4.d7b0ac4bd81058ada7ed526c7dc7fe5ca60b6b3e977964fb3a8f0e10cad178e8.e84a606188^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:27:29Z</t>
+  </si>
+  <si>
+    <t>ff473e48b4dcd130</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:29:30Z</t>
+  </si>
+  <si>
+    <t>dc92e7d1e3a746a9</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:12:25Z</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:16:36Z</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:18:00Z</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:19:35Z</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:20:57Z</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:22:01Z</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:23:31Z</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:24:46Z</t>
+  </si>
+  <si>
+    <t>2023-10-16T09:25:52Z</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1625,6 +1625,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1700,10 +1703,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4088,10 +4087,10 @@
   <dimension ref="A1:T378"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4206,7 +4205,7 @@
       <c r="A5" s="57"/>
       <c r="B5" s="58"/>
       <c r="C5" s="60" t="s">
-        <v>237</v>
+        <v>188</v>
       </c>
       <c r="D5" s="51"/>
       <c r="E5" s="45"/>
@@ -4362,13 +4361,13 @@
         <v>119</v>
       </c>
       <c r="F10" s="29">
-        <v>45202</v>
+        <v>45215</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>171</v>
+        <v>228</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>172</v>
+        <v>229</v>
       </c>
       <c r="I10" s="29" t="s">
         <v>113</v>
@@ -4418,13 +4417,13 @@
         <v>121</v>
       </c>
       <c r="F11" s="29">
-        <v>45202</v>
+        <v>45215</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>174</v>
+        <v>230</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>173</v>
+        <v>231</v>
       </c>
       <c r="I11" s="29" t="s">
         <v>113</v>
@@ -4674,16 +4673,16 @@
         <v>133</v>
       </c>
       <c r="F17" s="29">
-        <v>45202</v>
+        <v>45215</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="H17" s="36" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="I17" s="36" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="J17" s="30" t="s">
         <v>55</v>
@@ -4696,7 +4695,7 @@
         <v>55</v>
       </c>
       <c r="N17" s="30" t="s">
-        <v>222</v>
+        <v>173</v>
       </c>
       <c r="O17" s="30" t="s">
         <v>55</v>
@@ -4730,16 +4729,16 @@
         <v>135</v>
       </c>
       <c r="F18" s="29">
-        <v>45202</v>
+        <v>45215</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="H18" s="36" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="I18" s="36" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="J18" s="30" t="s">
         <v>55</v>
@@ -4752,7 +4751,7 @@
         <v>55</v>
       </c>
       <c r="N18" s="30" t="s">
-        <v>223</v>
+        <v>174</v>
       </c>
       <c r="O18" s="30" t="s">
         <v>55</v>
@@ -4786,16 +4785,16 @@
         <v>137</v>
       </c>
       <c r="F19" s="29">
-        <v>45202</v>
+        <v>45215</v>
       </c>
       <c r="G19" s="36" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="H19" s="36" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="J19" s="30" t="s">
         <v>55</v>
@@ -4808,7 +4807,7 @@
         <v>55</v>
       </c>
       <c r="N19" s="30" t="s">
-        <v>224</v>
+        <v>175</v>
       </c>
       <c r="O19" s="30" t="s">
         <v>55</v>
@@ -4842,16 +4841,16 @@
         <v>139</v>
       </c>
       <c r="F20" s="29">
-        <v>45202</v>
+        <v>45215</v>
       </c>
       <c r="G20" s="36" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="H20" s="36" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="I20" s="36" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="J20" s="30" t="s">
         <v>55</v>
@@ -4864,7 +4863,7 @@
         <v>55</v>
       </c>
       <c r="N20" s="30" t="s">
-        <v>225</v>
+        <v>176</v>
       </c>
       <c r="O20" s="30" t="s">
         <v>55</v>
@@ -4898,16 +4897,16 @@
         <v>141</v>
       </c>
       <c r="F21" s="29">
-        <v>45203</v>
-      </c>
-      <c r="G21" s="36" t="s">
-        <v>214</v>
+        <v>45215</v>
+      </c>
+      <c r="G21" s="61" t="s">
+        <v>232</v>
       </c>
       <c r="H21" s="36" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="J21" s="30" t="s">
         <v>55</v>
@@ -4920,7 +4919,7 @@
         <v>55</v>
       </c>
       <c r="N21" s="30" t="s">
-        <v>226</v>
+        <v>177</v>
       </c>
       <c r="O21" s="30" t="s">
         <v>55</v>
@@ -4954,16 +4953,16 @@
         <v>143</v>
       </c>
       <c r="F22" s="29">
-        <v>45203</v>
+        <v>45215</v>
       </c>
       <c r="G22" s="36" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H22" s="36" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="I22" s="36" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="J22" s="30" t="s">
         <v>55</v>
@@ -4976,7 +4975,7 @@
         <v>55</v>
       </c>
       <c r="N22" s="30" t="s">
-        <v>227</v>
+        <v>178</v>
       </c>
       <c r="O22" s="30" t="s">
         <v>55</v>
@@ -5010,16 +5009,16 @@
         <v>145</v>
       </c>
       <c r="F23" s="29">
-        <v>45203</v>
+        <v>45215</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H23" s="36" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="J23" s="30" t="s">
         <v>55</v>
@@ -5032,7 +5031,7 @@
         <v>55</v>
       </c>
       <c r="N23" s="30" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="O23" s="30" t="s">
         <v>55</v>
@@ -5066,16 +5065,16 @@
         <v>147</v>
       </c>
       <c r="F24" s="29">
-        <v>45203</v>
-      </c>
-      <c r="G24" s="36" t="s">
-        <v>217</v>
+        <v>45215</v>
+      </c>
+      <c r="G24" s="61" t="s">
+        <v>233</v>
       </c>
       <c r="H24" s="36" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="J24" s="30" t="s">
         <v>55</v>
@@ -5088,7 +5087,7 @@
         <v>55</v>
       </c>
       <c r="N24" s="30" t="s">
-        <v>229</v>
+        <v>180</v>
       </c>
       <c r="O24" s="30" t="s">
         <v>55</v>
@@ -5122,16 +5121,16 @@
         <v>149</v>
       </c>
       <c r="F25" s="29">
-        <v>45203</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>196</v>
+        <v>45215</v>
+      </c>
+      <c r="G25" s="61" t="s">
+        <v>234</v>
       </c>
       <c r="H25" s="36" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="I25" s="36" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="J25" s="30" t="s">
         <v>55</v>
@@ -5144,7 +5143,7 @@
         <v>55</v>
       </c>
       <c r="N25" s="30" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="O25" s="30" t="s">
         <v>55</v>
@@ -5178,16 +5177,16 @@
         <v>151</v>
       </c>
       <c r="F26" s="29">
-        <v>45203</v>
-      </c>
-      <c r="G26" s="36" t="s">
-        <v>218</v>
+        <v>45215</v>
+      </c>
+      <c r="G26" s="61" t="s">
+        <v>235</v>
       </c>
       <c r="H26" s="36" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="J26" s="30" t="s">
         <v>55</v>
@@ -5200,7 +5199,7 @@
         <v>55</v>
       </c>
       <c r="N26" s="30" t="s">
-        <v>231</v>
+        <v>182</v>
       </c>
       <c r="O26" s="30" t="s">
         <v>55</v>
@@ -5234,16 +5233,16 @@
         <v>153</v>
       </c>
       <c r="F27" s="29">
-        <v>45203</v>
-      </c>
-      <c r="G27" s="36" t="s">
+        <v>45215</v>
+      </c>
+      <c r="G27" s="61" t="s">
+        <v>236</v>
+      </c>
+      <c r="H27" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="I27" s="36" t="s">
         <v>219</v>
-      </c>
-      <c r="H27" s="36" t="s">
-        <v>199</v>
-      </c>
-      <c r="I27" s="36" t="s">
-        <v>200</v>
       </c>
       <c r="J27" s="30" t="s">
         <v>55</v>
@@ -5256,7 +5255,7 @@
         <v>55</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>232</v>
+        <v>183</v>
       </c>
       <c r="O27" s="30" t="s">
         <v>55</v>
@@ -5290,16 +5289,16 @@
         <v>155</v>
       </c>
       <c r="F28" s="29">
-        <v>45203</v>
-      </c>
-      <c r="G28" s="36" t="s">
+        <v>45215</v>
+      </c>
+      <c r="G28" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="H28" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="H28" s="36" t="s">
-        <v>201</v>
-      </c>
       <c r="I28" s="36" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
       <c r="J28" s="30" t="s">
         <v>55</v>
@@ -5312,7 +5311,7 @@
         <v>55</v>
       </c>
       <c r="N28" s="30" t="s">
-        <v>233</v>
+        <v>184</v>
       </c>
       <c r="O28" s="30" t="s">
         <v>55</v>
@@ -5346,16 +5345,16 @@
         <v>157</v>
       </c>
       <c r="F29" s="29">
-        <v>45203</v>
-      </c>
-      <c r="G29" s="36" t="s">
-        <v>221</v>
+        <v>45215</v>
+      </c>
+      <c r="G29" s="61" t="s">
+        <v>238</v>
       </c>
       <c r="H29" s="44" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="I29" s="44" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="J29" s="30" t="s">
         <v>55</v>
@@ -5368,7 +5367,7 @@
         <v>55</v>
       </c>
       <c r="N29" s="30" t="s">
-        <v>234</v>
+        <v>185</v>
       </c>
       <c r="O29" s="46" t="s">
         <v>55</v>
@@ -5553,17 +5552,17 @@
       <c r="E34" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="F34" s="29">
-        <v>45203</v>
-      </c>
-      <c r="G34" s="36" t="s">
-        <v>207</v>
+      <c r="F34" s="40">
+        <v>45215</v>
+      </c>
+      <c r="G34" s="61" t="s">
+        <v>239</v>
       </c>
       <c r="H34" s="36" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="I34" s="36" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="J34" s="30" t="s">
         <v>55</v>
@@ -5576,7 +5575,7 @@
         <v>55</v>
       </c>
       <c r="N34" s="30" t="s">
-        <v>235</v>
+        <v>186</v>
       </c>
       <c r="O34" s="30" t="s">
         <v>55</v>
@@ -5609,17 +5608,17 @@
       <c r="E35" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="F35" s="29">
-        <v>45203</v>
-      </c>
-      <c r="G35" s="36" t="s">
-        <v>210</v>
+      <c r="F35" s="40">
+        <v>45215</v>
+      </c>
+      <c r="G35" s="61" t="s">
+        <v>240</v>
       </c>
       <c r="H35" s="36" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="I35" s="36" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="J35" s="30" t="s">
         <v>55</v>
@@ -5632,7 +5631,7 @@
         <v>55</v>
       </c>
       <c r="N35" s="30" t="s">
-        <v>236</v>
+        <v>187</v>
       </c>
       <c r="O35" s="30" t="s">
         <v>55</v>
@@ -5660,22 +5659,22 @@
         <v>54</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F36" s="40">
-        <v>45202</v>
+        <v>45215</v>
       </c>
       <c r="G36" s="47" t="s">
-        <v>238</v>
+        <v>191</v>
       </c>
       <c r="H36" s="47" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
       <c r="I36" s="47" t="s">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="J36" s="25" t="s">
         <v>55</v>

</xml_diff>